<commit_message>
Decoder 1 Rev 1
</commit_message>
<xml_diff>
--- a/InstructionsSet.xlsx
+++ b/InstructionsSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\InfoLaptop\Bread80\Datapoint2200\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F918FF63-3210-4A50-BE83-31F5B00AE019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50599DE-6593-4B84-BCAF-A3565735982C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{166DEF7B-924A-48BF-9773-765780BBC1E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{166DEF7B-924A-48BF-9773-765780BBC1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="600">
   <si>
     <t>0x</t>
   </si>
@@ -3946,8 +3946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24128FF0-399B-47DA-9E9B-73395452F2CE}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4056,6 +4056,9 @@
       <c r="P4" s="2" t="s">
         <v>434</v>
       </c>
+      <c r="Q4" s="4" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -4082,6 +4085,9 @@
       <c r="H5" s="2" t="s">
         <v>439</v>
       </c>
+      <c r="I5" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="J5" s="3" t="s">
         <v>440</v>
       </c>
@@ -4102,6 +4108,9 @@
       </c>
       <c r="P5" s="2" t="s">
         <v>450</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -4126,6 +4135,9 @@
       <c r="H6" s="2" t="s">
         <v>446</v>
       </c>
+      <c r="I6" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="J6" s="3" t="s">
         <v>447</v>
       </c>
@@ -4143,6 +4155,9 @@
       </c>
       <c r="P6" s="2" t="s">
         <v>451</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4167,6 +4182,9 @@
       <c r="H7" s="2" t="s">
         <v>455</v>
       </c>
+      <c r="I7" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="M7" s="4" t="s">
         <v>46</v>
       </c>
@@ -4178,6 +4196,9 @@
       </c>
       <c r="P7" s="2" t="s">
         <v>457</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4970,7 +4991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF6E4C0-4B48-4C93-BC8E-AE98B938E13C}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>

</xml_diff>